<commit_message>
Trace et envoi de statements vers le LRS
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260"/>
+    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>URI</t>
   </si>
@@ -208,6 +208,30 @@
   </si>
   <si>
     <t>A dream fragment in the game E-LearningScape.</t>
+  </si>
+  <si>
+    <t>released</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/released</t>
+  </si>
+  <si>
+    <t>Indicates that the actor released the object from one's grip from or a specific state.</t>
+  </si>
+  <si>
+    <t>dragged</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/dragged</t>
+  </si>
+  <si>
+    <t>Indicates that the actor started dragging the object.</t>
+  </si>
+  <si>
+    <t>draggable</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/draggable</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1276,6 +1300,28 @@
       </c>
       <c r="C13" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1292,6 +1338,8 @@
     <hyperlink ref="B11" r:id="rId10"/>
     <hyperlink ref="B12" r:id="rId11"/>
     <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="B15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1551,10 +1599,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1668,6 +1716,14 @@
         <v>59</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1679,6 +1735,7 @@
     <hyperlink ref="B8" r:id="rId7"/>
     <hyperlink ref="B9" r:id="rId8"/>
     <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3250,6 +3307,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002AF8BD77682A724D8C3CDE17EF043D04" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0bf18f5715a3c32625528aa9cf69777">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb470b12-e12f-4a6c-8c4e-b69976333524" xmlns:ns3="35b094a4-12a1-4fa9-8f69-05d08f840d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0ac61fa3f519b84257a19b7fcabbdac" ns2:_="" ns3:_="">
     <xsd:import namespace="bb470b12-e12f-4a6c-8c4e-b69976333524"/>
@@ -3420,22 +3492,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB0AA923-8FEF-4C78-9E38-5BD5DFE72B3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3452,21 +3526,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correction de bugs traces et RdP
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>URI</t>
   </si>
@@ -39,55 +39,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>started</t>
-  </si>
-  <si>
-    <t>serious-game</t>
-  </si>
-  <si>
-    <t>A game designed for a primary purpose other than pure entertainment. For instance, an educational game or a game-like simulation. A serious game is the root container for the rest of game elements.</t>
-  </si>
-  <si>
     <t>collected</t>
   </si>
   <si>
     <t>https://www.lip6.fr/mocah/invalidURI/verbs/collected</t>
-  </si>
-  <si>
-    <t>interacted</t>
-  </si>
-  <si>
-    <t>Indicates the actor engaged with a physical or virtual object.</t>
-  </si>
-  <si>
-    <t>completed</t>
-  </si>
-  <si>
-    <t>accessed</t>
-  </si>
-  <si>
-    <t>unlocked</t>
-  </si>
-  <si>
-    <t>Indicates the actor unlocked an option that was previously unavailable. Used when the player unlocks an option in an alternative.</t>
-  </si>
-  <si>
-    <t>answered</t>
-  </si>
-  <si>
-    <t>Indicates the actor replied to a question, where the object is generally an activity representing the question.</t>
-  </si>
-  <si>
-    <t>exited</t>
-  </si>
-  <si>
-    <t>Indicates the actor intentionally departed from the activity or object.</t>
-  </si>
-  <si>
-    <t>pressed</t>
-  </si>
-  <si>
-    <t>Indicates that the actor made physical contact with the object. Used when the player presses some button in an input device. Press the left button in a mouse, press the X button in a XBox controller, etc.</t>
   </si>
   <si>
     <t>activated</t>
@@ -99,67 +54,16 @@
     <t>deactivated</t>
   </si>
   <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/interacted</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/completed</t>
-  </si>
-  <si>
     <t>https://www.lip6.fr/mocah/invalidURI/verbs/activated</t>
   </si>
   <si>
     <t>https://www.lip6.fr/mocah/invalidURI/verbs/deactivated</t>
   </si>
   <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/accessed</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/exited</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/unlocked</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/answered</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/started</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/pressed</t>
-  </si>
-  <si>
-    <t>Indicates that the actor accesses to the object. Associated to the virtual places a player visits during a gameplay.</t>
-  </si>
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>A question is typically part of an assessment and requires a response from the learner, a response that is then evaluated for correctness.</t>
-  </si>
-  <si>
-    <t>item</t>
-  </si>
-  <si>
-    <t>A collectable game object whose use or interaction results in an effect in a game. Items are common elements in video games. Players can collect/use/combine them.</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>An identified area inside the game world. In some games they can also be worlds. Represents an aggregation of zones.</t>
-  </si>
-  <si>
     <t>toggable</t>
   </si>
   <si>
     <t>interactable</t>
-  </si>
-  <si>
-    <t>menu</t>
-  </si>
-  <si>
-    <t>A menu with several buttons/options whose selection produces different effects. Represents a menu, integrated in the user interface (UI), with several a options.</t>
   </si>
   <si>
     <t>key</t>
@@ -177,9 +81,6 @@
     <t>Indicates that the actor put its cursor over the object.</t>
   </si>
   <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/serious-game</t>
-  </si>
-  <si>
     <t>https://www.lip6.fr/mocah/invalidURI/activity-types/toggable</t>
   </si>
   <si>
@@ -190,18 +91,6 @@
   </si>
   <si>
     <t>https://www.lip6.fr/mocah/invalidURI/activity-types/fragment</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/question</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/item</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/area</t>
-  </si>
-  <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/menu</t>
   </si>
   <si>
     <t>A keyboard or mouse key.</t>
@@ -1158,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1184,162 +1073,81 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B5" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
-    <hyperlink ref="B7" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1599,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1625,103 +1433,48 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1731,11 +1484,6 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3307,18 +3055,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3493,18 +3241,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Liste d'éléments tracés complétée + extensions dans ActionPerformedForLRS
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260" activeTab="1"/>
+    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>URI</t>
   </si>
@@ -69,9 +69,6 @@
     <t>key</t>
   </si>
   <si>
-    <t>fragment</t>
-  </si>
-  <si>
     <t>highlighted</t>
   </si>
   <si>
@@ -90,30 +87,15 @@
     <t>https://www.lip6.fr/mocah/invalidURI/activity-types/key</t>
   </si>
   <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/fragment</t>
-  </si>
-  <si>
     <t>A keyboard or mouse key.</t>
   </si>
   <si>
-    <t>A dream fragment in the game E-LearningScape.</t>
-  </si>
-  <si>
-    <t>released</t>
-  </si>
-  <si>
     <t>https://www.lip6.fr/mocah/invalidURI/verbs/released</t>
   </si>
   <si>
-    <t>Indicates that the actor released the object from one's grip from or a specific state.</t>
-  </si>
-  <si>
     <t>dragged</t>
   </si>
   <si>
-    <t>https://www.lip6.fr/mocah/invalidURI/verbs/dragged</t>
-  </si>
-  <si>
     <t>Indicates that the actor started dragging the object.</t>
   </si>
   <si>
@@ -121,6 +103,144 @@
   </si>
   <si>
     <t>https://www.lip6.fr/mocah/invalidURI/activity-types/draggable</t>
+  </si>
+  <si>
+    <t>skipped</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/skipped</t>
+  </si>
+  <si>
+    <t>viewable</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/viewable</t>
+  </si>
+  <si>
+    <t>crouched</t>
+  </si>
+  <si>
+    <t>stood</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/crouched</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/stood</t>
+  </si>
+  <si>
+    <t>moved</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/moved</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/avatar</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/received</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/feedback</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/type</t>
+  </si>
+  <si>
+    <t>dropped</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/dropped</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>animation</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/text</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/activity-types/animation</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/link</t>
+  </si>
+  <si>
+    <t>received</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/content</t>
+  </si>
+  <si>
+    <t>exitedHighlight</t>
+  </si>
+  <si>
+    <t>exitedView</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/exitedHighlight</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/exitedView</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/direction</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/value</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/position</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/state</t>
+  </si>
+  <si>
+    <t>attempted</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/attempted</t>
+  </si>
+  <si>
+    <t>reached</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/reached</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/time</t>
   </si>
 </sst>
 </file>
@@ -1047,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1100,45 +1220,105 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1148,6 +1328,15 @@
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
     <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="B16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1407,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1625,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1444,7 +1633,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1452,29 +1641,58 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1484,6 +1702,10 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1491,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1737,81 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3055,21 +3351,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002AF8BD77682A724D8C3CDE17EF043D04" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0bf18f5715a3c32625528aa9cf69777">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb470b12-e12f-4a6c-8c4e-b69976333524" xmlns:ns3="35b094a4-12a1-4fa9-8f69-05d08f840d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0ac61fa3f519b84257a19b7fcabbdac" ns2:_="" ns3:_="">
     <xsd:import namespace="bb470b12-e12f-4a6c-8c4e-b69976333524"/>
@@ -3240,24 +3521,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB0AA923-8FEF-4C78-9E38-5BD5DFE72B3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3274,4 +3553,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Save unsent statements + Remove extensions in statements
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -9,19 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260" activeTab="2"/>
+    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="8" r:id="rId1"/>
     <sheet name="Activity" sheetId="9" r:id="rId2"/>
     <sheet name="Extension" sheetId="10" r:id="rId3"/>
-    <sheet name="Grade" sheetId="11" r:id="rId4"/>
-    <sheet name="Domain" sheetId="1" r:id="rId5"/>
-    <sheet name="Subdomain" sheetId="3" r:id="rId6"/>
-    <sheet name="Skills" sheetId="4" r:id="rId7"/>
-    <sheet name="Topic" sheetId="5" r:id="rId8"/>
-    <sheet name="Focus" sheetId="6" r:id="rId9"/>
-    <sheet name="Action" sheetId="7" r:id="rId10"/>
+    <sheet name="Time" sheetId="19" r:id="rId4"/>
+    <sheet name="State" sheetId="18" r:id="rId5"/>
+    <sheet name="Position" sheetId="17" r:id="rId6"/>
+    <sheet name="Value" sheetId="16" r:id="rId7"/>
+    <sheet name="Direction" sheetId="15" r:id="rId8"/>
+    <sheet name="Content" sheetId="14" r:id="rId9"/>
+    <sheet name="Link" sheetId="13" r:id="rId10"/>
+    <sheet name="Type" sheetId="12" r:id="rId11"/>
+    <sheet name="Grade" sheetId="11" r:id="rId12"/>
+    <sheet name="Domain" sheetId="1" r:id="rId13"/>
+    <sheet name="Subdomain" sheetId="3" r:id="rId14"/>
+    <sheet name="Skills" sheetId="4" r:id="rId15"/>
+    <sheet name="Topic" sheetId="5" r:id="rId16"/>
+    <sheet name="Focus" sheetId="6" r:id="rId17"/>
+    <sheet name="Action" sheetId="7" r:id="rId18"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1345,478 +1353,29 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="213" workbookViewId="0">
-      <selection activeCell="B4" sqref="B3:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
-    <col min="2" max="2" width="33.875" customWidth="1"/>
-    <col min="3" max="3" width="135" customWidth="1"/>
-    <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="5.625" customWidth="1"/>
-    <col min="6" max="6" width="28.375" customWidth="1"/>
-    <col min="7" max="7" width="26.875" customWidth="1"/>
-    <col min="8" max="8" width="61.625" customWidth="1"/>
-    <col min="9" max="9" width="64.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="4.875" customWidth="1"/>
-    <col min="12" max="13" width="4.375" customWidth="1"/>
-    <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="15" max="15" width="4.375" customWidth="1"/>
-    <col min="16" max="16" width="4.625" customWidth="1"/>
-    <col min="17" max="17" width="42" customWidth="1"/>
-    <col min="18" max="18" width="3.125" customWidth="1"/>
-    <col min="19" max="19" width="3.375" customWidth="1"/>
-    <col min="20" max="20" width="44.125" customWidth="1"/>
-    <col min="21" max="21" width="15.625" customWidth="1"/>
-    <col min="22" max="22" width="6.5" customWidth="1"/>
-    <col min="23" max="23" width="25.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H2" s="2"/>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H3" s="2"/>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="2"/>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H5" s="2"/>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H6" s="2"/>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H7" s="2"/>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H9" s="2"/>
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H10" s="2"/>
-      <c r="I10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="2"/>
-      <c r="I12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H13" s="2"/>
-      <c r="I13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="2"/>
-      <c r="I15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H16" s="2"/>
-      <c r="I16"/>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H17" s="2"/>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="2"/>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="2"/>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="2"/>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H21" s="2"/>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H22" s="2"/>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H23" s="2"/>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H25" s="2"/>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H26" s="2"/>
-      <c r="I26"/>
-    </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H27" s="2"/>
-      <c r="I27"/>
-    </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="I28"/>
-    </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="I29"/>
-    </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="I30"/>
-    </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H31" s="2"/>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H32" s="2"/>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H33" s="2"/>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H34" s="2"/>
-      <c r="I34"/>
-    </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H35" s="2"/>
-      <c r="I35"/>
-    </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H36" s="2"/>
-      <c r="I36"/>
-    </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H37" s="2"/>
-      <c r="I37"/>
-    </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="2"/>
-      <c r="I38"/>
-    </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H39" s="2"/>
-      <c r="I39"/>
-    </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H40" s="2"/>
-      <c r="I40"/>
-    </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H41" s="2"/>
-      <c r="I41"/>
-    </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H42" s="2"/>
-      <c r="I42"/>
-    </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H43" s="2"/>
-      <c r="I43"/>
-    </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H44" s="2"/>
-      <c r="I44"/>
-    </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H45" s="2"/>
-      <c r="I45"/>
-    </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H46" s="2"/>
-      <c r="I46"/>
-    </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H47" s="2"/>
-      <c r="I47"/>
-    </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H48" s="2"/>
-      <c r="I48"/>
-    </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H49" s="2"/>
-      <c r="I49"/>
-    </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H50" s="2"/>
-      <c r="I50"/>
-    </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H51" s="2"/>
-      <c r="I51"/>
-    </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H52" s="2"/>
-      <c r="I52"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="H2:H52">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.375" customWidth="1"/>
-    <col min="2" max="2" width="35.625" customWidth="1"/>
-    <col min="3" max="3" width="168.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-  </hyperlinks>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.125" customWidth="1"/>
-    <col min="2" max="2" width="36.125" customWidth="1"/>
-    <col min="3" max="3" width="158.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-  </hyperlinks>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -1847,7 +1406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
@@ -2021,7 +1580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
@@ -2198,7 +1757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
@@ -2468,7 +2027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I112"/>
   <sheetViews>
@@ -2858,7 +2417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I145"/>
   <sheetViews>
@@ -3347,6 +2906,551 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView zoomScale="112" zoomScaleNormal="213" workbookViewId="0">
+      <selection activeCell="B4" sqref="B3:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="33.875" customWidth="1"/>
+    <col min="3" max="3" width="135" customWidth="1"/>
+    <col min="4" max="4" width="3.5" customWidth="1"/>
+    <col min="5" max="5" width="5.625" customWidth="1"/>
+    <col min="6" max="6" width="28.375" customWidth="1"/>
+    <col min="7" max="7" width="26.875" customWidth="1"/>
+    <col min="8" max="8" width="61.625" customWidth="1"/>
+    <col min="9" max="9" width="64.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
+    <col min="11" max="11" width="4.875" customWidth="1"/>
+    <col min="12" max="13" width="4.375" customWidth="1"/>
+    <col min="14" max="14" width="5" customWidth="1"/>
+    <col min="15" max="15" width="4.375" customWidth="1"/>
+    <col min="16" max="16" width="4.625" customWidth="1"/>
+    <col min="17" max="17" width="42" customWidth="1"/>
+    <col min="18" max="18" width="3.125" customWidth="1"/>
+    <col min="19" max="19" width="3.375" customWidth="1"/>
+    <col min="20" max="20" width="44.125" customWidth="1"/>
+    <col min="21" max="21" width="15.625" customWidth="1"/>
+    <col min="22" max="22" width="6.5" customWidth="1"/>
+    <col min="23" max="23" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="2"/>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="2"/>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="2"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="2"/>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+      <c r="I13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+      <c r="I19"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I29"/>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I30"/>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="2"/>
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+      <c r="I36"/>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="2"/>
+      <c r="I37"/>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H38" s="2"/>
+      <c r="I38"/>
+    </row>
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H39" s="2"/>
+      <c r="I39"/>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+      <c r="I40"/>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="2"/>
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="2"/>
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="I44"/>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="I45"/>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="2"/>
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H47" s="2"/>
+      <c r="I47"/>
+    </row>
+    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="2"/>
+      <c r="I48"/>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H49" s="2"/>
+      <c r="I49"/>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H50" s="2"/>
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H51" s="2"/>
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H52" s="2"/>
+      <c r="I52"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H2:H52">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.375" customWidth="1"/>
+    <col min="2" max="2" width="35.625" customWidth="1"/>
+    <col min="3" max="3" width="168.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.125" customWidth="1"/>
+    <col min="2" max="2" width="36.125" customWidth="1"/>
+    <col min="3" max="3" width="158.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3522,18 +3626,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3556,18 +3660,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tracer HelpSystem vers le LRS + MaJ champ "Authorization" GBLXAPI
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
   <si>
     <t>URI</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>https://www.lip6.fr/mocah/invalidURI/extensions/time</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/from</t>
   </si>
 </sst>
 </file>
@@ -3279,10 +3285,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3367,6 +3373,14 @@
         <v>70</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -3377,6 +3391,7 @@
     <hyperlink ref="B7" r:id="rId6"/>
     <hyperlink ref="B8" r:id="rId7"/>
     <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3386,7 +3401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -3455,6 +3470,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002AF8BD77682A724D8C3CDE17EF043D04" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0bf18f5715a3c32625528aa9cf69777">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb470b12-e12f-4a6c-8c4e-b69976333524" xmlns:ns3="35b094a4-12a1-4fa9-8f69-05d08f840d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0ac61fa3f519b84257a19b7fcabbdac" ns2:_="" ns3:_="">
     <xsd:import namespace="bb470b12-e12f-4a6c-8c4e-b69976333524"/>
@@ -3625,22 +3655,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB0AA923-8FEF-4C78-9E38-5BD5DFE72B3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3657,21 +3689,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correction du composant wrapper manquant + activation aléatoire HelpSystem + modification traces IARDreamFragmentManager
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mounswif\LearningScape\Vocabulary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents HDD\LearningScape\LearningScape\Vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5FEEF2-62C1-4429-949B-A24F0E8EBA52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="465" windowWidth="27600" windowHeight="16260" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="8" r:id="rId1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>URI</t>
   </si>
@@ -255,12 +256,24 @@
   </si>
   <si>
     <t>https://www.lip6.fr/mocah/invalidURI/extensions/from</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/rotation</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/scale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1180,21 +1193,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="34.125" customWidth="1"/>
-    <col min="3" max="3" width="163.875" customWidth="1"/>
+    <col min="2" max="2" width="34.09765625" customWidth="1"/>
+    <col min="3" max="3" width="163.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1205,7 +1218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1216,7 +1229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1224,7 +1237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1232,7 +1245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1243,7 +1256,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1251,7 +1264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1262,7 +1275,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1270,7 +1283,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1278,7 +1291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1286,7 +1299,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1294,7 +1307,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1302,7 +1315,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1310,7 +1323,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1318,7 +1331,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1326,7 +1339,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1336,21 +1349,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1358,45 +1371,45 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
     <col min="3" max="3" width="140" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1413,40 +1426,40 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="213" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.375" customWidth="1"/>
+    <col min="1" max="1" width="39.3984375" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
     <col min="3" max="3" width="96.5" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="10.625" customWidth="1"/>
-    <col min="6" max="6" width="30.625" customWidth="1"/>
-    <col min="7" max="7" width="27.875" customWidth="1"/>
-    <col min="8" max="8" width="50.625" customWidth="1"/>
-    <col min="9" max="9" width="87.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="4.875" customWidth="1"/>
-    <col min="12" max="13" width="4.375" customWidth="1"/>
-    <col min="14" max="14" width="7.375" customWidth="1"/>
-    <col min="15" max="15" width="4.375" customWidth="1"/>
-    <col min="16" max="16" width="4.625" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" customWidth="1"/>
+    <col min="6" max="6" width="30.59765625" customWidth="1"/>
+    <col min="7" max="7" width="27.8984375" customWidth="1"/>
+    <col min="8" max="8" width="50.59765625" customWidth="1"/>
+    <col min="9" max="9" width="87.8984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.8984375" customWidth="1"/>
+    <col min="11" max="11" width="4.8984375" customWidth="1"/>
+    <col min="12" max="13" width="4.3984375" customWidth="1"/>
+    <col min="14" max="14" width="7.3984375" customWidth="1"/>
+    <col min="15" max="15" width="4.3984375" customWidth="1"/>
+    <col min="16" max="16" width="4.59765625" customWidth="1"/>
     <col min="17" max="17" width="42" customWidth="1"/>
-    <col min="18" max="18" width="3.125" customWidth="1"/>
-    <col min="19" max="19" width="3.375" customWidth="1"/>
-    <col min="20" max="20" width="44.125" customWidth="1"/>
-    <col min="21" max="21" width="15.625" customWidth="1"/>
+    <col min="18" max="18" width="3.09765625" customWidth="1"/>
+    <col min="19" max="19" width="3.3984375" customWidth="1"/>
+    <col min="20" max="20" width="44.09765625" customWidth="1"/>
+    <col min="21" max="21" width="15.59765625" customWidth="1"/>
     <col min="22" max="22" width="6.5" customWidth="1"/>
     <col min="23" max="23" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1457,124 +1470,124 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I18"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20"/>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I22"/>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I23"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I24"/>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I25"/>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I26"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I27"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I28"/>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I29"/>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I30"/>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I31"/>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I32"/>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I33"/>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I34"/>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I35"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I36"/>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I37"/>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I38"/>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I39"/>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I40"/>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I41"/>
     </row>
   </sheetData>
@@ -1587,40 +1600,40 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="213" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.375" customWidth="1"/>
-    <col min="2" max="2" width="46.375" customWidth="1"/>
+    <col min="1" max="1" width="41.3984375" customWidth="1"/>
+    <col min="2" max="2" width="46.3984375" customWidth="1"/>
     <col min="3" max="3" width="111" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="5.59765625" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
-    <col min="7" max="7" width="31.375" customWidth="1"/>
-    <col min="8" max="8" width="50.625" customWidth="1"/>
-    <col min="9" max="9" width="87.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="4.875" customWidth="1"/>
-    <col min="12" max="13" width="4.375" customWidth="1"/>
-    <col min="14" max="14" width="7.375" customWidth="1"/>
-    <col min="15" max="15" width="4.375" customWidth="1"/>
-    <col min="16" max="16" width="4.625" customWidth="1"/>
+    <col min="7" max="7" width="31.3984375" customWidth="1"/>
+    <col min="8" max="8" width="50.59765625" customWidth="1"/>
+    <col min="9" max="9" width="87.8984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.8984375" customWidth="1"/>
+    <col min="11" max="11" width="4.8984375" customWidth="1"/>
+    <col min="12" max="13" width="4.3984375" customWidth="1"/>
+    <col min="14" max="14" width="7.3984375" customWidth="1"/>
+    <col min="15" max="15" width="4.3984375" customWidth="1"/>
+    <col min="16" max="16" width="4.59765625" customWidth="1"/>
     <col min="17" max="17" width="42" customWidth="1"/>
-    <col min="18" max="18" width="3.125" customWidth="1"/>
-    <col min="19" max="19" width="3.375" customWidth="1"/>
-    <col min="20" max="20" width="44.125" customWidth="1"/>
-    <col min="21" max="21" width="15.625" customWidth="1"/>
+    <col min="18" max="18" width="3.09765625" customWidth="1"/>
+    <col min="19" max="19" width="3.3984375" customWidth="1"/>
+    <col min="20" max="20" width="44.09765625" customWidth="1"/>
+    <col min="21" max="21" width="15.59765625" customWidth="1"/>
     <col min="22" max="22" width="6.5" customWidth="1"/>
     <col min="23" max="23" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1631,128 +1644,128 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I18"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20"/>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I22"/>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I23"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I24"/>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I25"/>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I26"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I27"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I28"/>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I29"/>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I30"/>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I31"/>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I32"/>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I33"/>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I34"/>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I35"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I36"/>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I37"/>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I38"/>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I39"/>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I40"/>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I41"/>
     </row>
   </sheetData>
-  <sortState ref="A2:W40">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W40">
     <sortCondition ref="F2:F40"/>
   </sortState>
   <conditionalFormatting sqref="H2:H40">
@@ -1764,40 +1777,40 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView zoomScaleNormal="213" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.875" customWidth="1"/>
-    <col min="2" max="2" width="51.375" customWidth="1"/>
-    <col min="3" max="3" width="144.125" customWidth="1"/>
+    <col min="1" max="1" width="29.8984375" customWidth="1"/>
+    <col min="2" max="2" width="51.3984375" customWidth="1"/>
+    <col min="3" max="3" width="144.09765625" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="5.59765625" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
-    <col min="7" max="7" width="34.875" customWidth="1"/>
-    <col min="8" max="8" width="50.625" customWidth="1"/>
-    <col min="9" max="9" width="87.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="4.875" customWidth="1"/>
-    <col min="12" max="13" width="4.375" customWidth="1"/>
-    <col min="14" max="14" width="7.375" customWidth="1"/>
-    <col min="15" max="15" width="4.375" customWidth="1"/>
-    <col min="16" max="16" width="4.625" customWidth="1"/>
+    <col min="7" max="7" width="34.8984375" customWidth="1"/>
+    <col min="8" max="8" width="50.59765625" customWidth="1"/>
+    <col min="9" max="9" width="87.8984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.8984375" customWidth="1"/>
+    <col min="11" max="11" width="4.8984375" customWidth="1"/>
+    <col min="12" max="13" width="4.3984375" customWidth="1"/>
+    <col min="14" max="14" width="7.3984375" customWidth="1"/>
+    <col min="15" max="15" width="4.3984375" customWidth="1"/>
+    <col min="16" max="16" width="4.59765625" customWidth="1"/>
     <col min="17" max="17" width="42" customWidth="1"/>
-    <col min="18" max="18" width="3.125" customWidth="1"/>
-    <col min="19" max="19" width="3.375" customWidth="1"/>
-    <col min="20" max="20" width="44.125" customWidth="1"/>
-    <col min="21" max="21" width="15.625" customWidth="1"/>
+    <col min="18" max="18" width="3.09765625" customWidth="1"/>
+    <col min="19" max="19" width="3.3984375" customWidth="1"/>
+    <col min="20" max="20" width="44.09765625" customWidth="1"/>
+    <col min="21" max="21" width="15.59765625" customWidth="1"/>
     <col min="22" max="22" width="6.5" customWidth="1"/>
     <col min="23" max="23" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1808,220 +1821,220 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H5" s="2"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H15" s="2"/>
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I18"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20"/>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I22"/>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I23"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I24"/>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I25"/>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I26"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I27"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I28"/>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I29"/>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I30"/>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I31"/>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I32"/>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I33"/>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I34"/>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I35"/>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I36"/>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I37"/>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I38"/>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39" s="2"/>
       <c r="I39"/>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I40"/>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I41"/>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I42"/>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I43"/>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I44"/>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I45"/>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I46"/>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I47"/>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I48"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I49"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I50"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I51"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I52"/>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I53"/>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I54"/>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I55"/>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I56"/>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I57"/>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I58"/>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I59"/>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I60"/>
     </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I61"/>
     </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I62"/>
     </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I63"/>
     </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I64"/>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I65"/>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I66"/>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I67"/>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I68"/>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I69"/>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I70"/>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I71"/>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I72"/>
     </row>
   </sheetData>
@@ -2034,40 +2047,40 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView zoomScale="111" zoomScaleNormal="213" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
-    <col min="2" max="2" width="45.125" customWidth="1"/>
-    <col min="3" max="3" width="124.375" customWidth="1"/>
+    <col min="2" max="2" width="45.09765625" customWidth="1"/>
+    <col min="3" max="3" width="124.3984375" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="5.625" customWidth="1"/>
-    <col min="6" max="6" width="45.125" customWidth="1"/>
-    <col min="7" max="7" width="34.875" customWidth="1"/>
-    <col min="8" max="8" width="50.625" customWidth="1"/>
-    <col min="9" max="9" width="87.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="4.875" customWidth="1"/>
-    <col min="12" max="13" width="4.375" customWidth="1"/>
-    <col min="14" max="14" width="7.375" customWidth="1"/>
-    <col min="15" max="15" width="4.375" customWidth="1"/>
-    <col min="16" max="16" width="4.625" customWidth="1"/>
+    <col min="5" max="5" width="5.59765625" customWidth="1"/>
+    <col min="6" max="6" width="45.09765625" customWidth="1"/>
+    <col min="7" max="7" width="34.8984375" customWidth="1"/>
+    <col min="8" max="8" width="50.59765625" customWidth="1"/>
+    <col min="9" max="9" width="87.8984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.8984375" customWidth="1"/>
+    <col min="11" max="11" width="4.8984375" customWidth="1"/>
+    <col min="12" max="13" width="4.3984375" customWidth="1"/>
+    <col min="14" max="14" width="7.3984375" customWidth="1"/>
+    <col min="15" max="15" width="4.3984375" customWidth="1"/>
+    <col min="16" max="16" width="4.59765625" customWidth="1"/>
     <col min="17" max="17" width="37" customWidth="1"/>
-    <col min="18" max="18" width="3.125" customWidth="1"/>
-    <col min="19" max="19" width="3.375" customWidth="1"/>
-    <col min="20" max="20" width="44.125" customWidth="1"/>
-    <col min="21" max="21" width="15.625" customWidth="1"/>
+    <col min="18" max="18" width="3.09765625" customWidth="1"/>
+    <col min="19" max="19" width="3.3984375" customWidth="1"/>
+    <col min="20" max="20" width="44.09765625" customWidth="1"/>
+    <col min="21" max="21" width="15.59765625" customWidth="1"/>
     <col min="22" max="22" width="6.5" customWidth="1"/>
     <col min="23" max="23" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2078,337 +2091,337 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I18"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20"/>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I22"/>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I23"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I24"/>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I25"/>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I26"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I27"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I28"/>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I29"/>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I30"/>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I31"/>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I32"/>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I33"/>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I34"/>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I35"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I36"/>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I37"/>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I38"/>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I39"/>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I40"/>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I41"/>
     </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I42"/>
     </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I43"/>
     </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I44"/>
     </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I45"/>
     </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I46"/>
     </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I47"/>
     </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I48"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I49"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I50"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I51"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I52"/>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I53"/>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I54"/>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I55"/>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I56"/>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I57"/>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I58"/>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I59"/>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I60"/>
     </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I61"/>
     </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I62"/>
     </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I63"/>
     </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I64"/>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I65"/>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I66"/>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I67"/>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I68"/>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I69"/>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I70"/>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I71"/>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I72"/>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I73"/>
     </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I74"/>
     </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I75"/>
     </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I76"/>
     </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I77"/>
     </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I78"/>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I79"/>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I80"/>
     </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I81"/>
     </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I82"/>
     </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I83"/>
     </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I84"/>
     </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I85"/>
     </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I86"/>
     </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I87"/>
     </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I88"/>
     </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I89"/>
     </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I90"/>
     </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I91"/>
     </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I92"/>
     </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I93"/>
     </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I94"/>
     </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I95"/>
     </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I96"/>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I97"/>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I98"/>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I99"/>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I100"/>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I101"/>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I102"/>
     </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I103"/>
     </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I104"/>
     </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I105"/>
     </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I106"/>
     </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I107"/>
     </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I108"/>
     </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I109"/>
     </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I110"/>
     </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I111"/>
     </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I112"/>
     </row>
   </sheetData>
@@ -2424,40 +2437,40 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:I145"/>
   <sheetViews>
     <sheetView zoomScaleNormal="213" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.375" customWidth="1"/>
+    <col min="1" max="1" width="29.3984375" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="154.375" customWidth="1"/>
+    <col min="3" max="3" width="154.3984375" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="5.59765625" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="50.625" customWidth="1"/>
-    <col min="9" max="9" width="87.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="4.875" customWidth="1"/>
-    <col min="12" max="13" width="4.375" customWidth="1"/>
-    <col min="14" max="14" width="7.375" customWidth="1"/>
-    <col min="15" max="15" width="4.375" customWidth="1"/>
-    <col min="16" max="16" width="4.625" customWidth="1"/>
+    <col min="8" max="8" width="50.59765625" customWidth="1"/>
+    <col min="9" max="9" width="87.8984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.8984375" customWidth="1"/>
+    <col min="11" max="11" width="4.8984375" customWidth="1"/>
+    <col min="12" max="13" width="4.3984375" customWidth="1"/>
+    <col min="14" max="14" width="7.3984375" customWidth="1"/>
+    <col min="15" max="15" width="4.3984375" customWidth="1"/>
+    <col min="16" max="16" width="4.59765625" customWidth="1"/>
     <col min="17" max="17" width="42" customWidth="1"/>
-    <col min="18" max="18" width="3.125" customWidth="1"/>
-    <col min="19" max="19" width="3.375" customWidth="1"/>
-    <col min="20" max="20" width="44.125" customWidth="1"/>
-    <col min="21" max="21" width="15.625" customWidth="1"/>
+    <col min="18" max="18" width="3.09765625" customWidth="1"/>
+    <col min="19" max="19" width="3.3984375" customWidth="1"/>
+    <col min="20" max="20" width="44.09765625" customWidth="1"/>
+    <col min="21" max="21" width="15.59765625" customWidth="1"/>
     <col min="22" max="22" width="6.5" customWidth="1"/>
     <col min="23" max="23" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2468,442 +2481,442 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H12" s="2"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I17"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I18"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I19"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I20"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I21"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I22"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="2"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I24"/>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I25"/>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I26"/>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I27"/>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I28"/>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="2"/>
       <c r="I29"/>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I30"/>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I31"/>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I32"/>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I33"/>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I34"/>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I35"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I36"/>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I37"/>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I38"/>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I39"/>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I40"/>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I41"/>
     </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I42"/>
     </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I43"/>
     </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I44"/>
     </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I45"/>
     </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I46"/>
     </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I47"/>
     </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I48"/>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I49"/>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I50"/>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I51"/>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H52" s="2"/>
       <c r="I52"/>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I53"/>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I54"/>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I55"/>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I56"/>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I57"/>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I58"/>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I59"/>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I60"/>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I61"/>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I62"/>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I63"/>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I64"/>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I65"/>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I66"/>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I67"/>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I68"/>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I69"/>
     </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I70"/>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I71"/>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I72"/>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I73"/>
     </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I74"/>
     </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I75"/>
     </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I76"/>
     </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I77"/>
     </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I78"/>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I79"/>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I80"/>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I81"/>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I82"/>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I83"/>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I84"/>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I85"/>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I86"/>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H87" s="2"/>
       <c r="I87"/>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I88"/>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I89"/>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I90"/>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I91"/>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I92"/>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I93"/>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I94"/>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I95"/>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I96"/>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I97"/>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I98"/>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I99"/>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I100"/>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I101"/>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I102"/>
     </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I103"/>
     </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I104"/>
     </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I105"/>
     </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I106"/>
     </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I107"/>
     </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I108"/>
     </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I109"/>
     </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I110"/>
     </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I111"/>
     </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I112"/>
     </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I113"/>
     </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I114"/>
     </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I115"/>
     </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I116"/>
     </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I117"/>
     </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I118"/>
     </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I119"/>
     </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I120"/>
     </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I121"/>
     </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I122"/>
     </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I123"/>
     </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I124"/>
     </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I125"/>
     </row>
-    <row r="126" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I126"/>
     </row>
-    <row r="127" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I127"/>
     </row>
-    <row r="128" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I128"/>
     </row>
-    <row r="129" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I129"/>
     </row>
-    <row r="130" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I130"/>
     </row>
-    <row r="131" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I131"/>
     </row>
-    <row r="132" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I132"/>
     </row>
-    <row r="133" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I133"/>
     </row>
-    <row r="134" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I134"/>
     </row>
-    <row r="135" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H135" s="2"/>
       <c r="I135"/>
     </row>
-    <row r="136" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I136"/>
     </row>
-    <row r="137" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I137"/>
     </row>
-    <row r="138" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I138"/>
     </row>
-    <row r="139" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I139"/>
     </row>
-    <row r="140" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I140"/>
     </row>
-    <row r="141" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I141"/>
     </row>
-    <row r="142" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I142"/>
     </row>
-    <row r="143" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I143"/>
     </row>
-    <row r="144" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I144"/>
     </row>
-    <row r="145" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I145"/>
     </row>
   </sheetData>
@@ -2916,40 +2929,40 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="213" workbookViewId="0">
       <selection activeCell="B4" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.5" customWidth="1"/>
-    <col min="2" max="2" width="33.875" customWidth="1"/>
+    <col min="2" max="2" width="33.8984375" customWidth="1"/>
     <col min="3" max="3" width="135" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="5.625" customWidth="1"/>
-    <col min="6" max="6" width="28.375" customWidth="1"/>
-    <col min="7" max="7" width="26.875" customWidth="1"/>
-    <col min="8" max="8" width="61.625" customWidth="1"/>
-    <col min="9" max="9" width="64.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" customWidth="1"/>
-    <col min="11" max="11" width="4.875" customWidth="1"/>
-    <col min="12" max="13" width="4.375" customWidth="1"/>
+    <col min="5" max="5" width="5.59765625" customWidth="1"/>
+    <col min="6" max="6" width="28.3984375" customWidth="1"/>
+    <col min="7" max="7" width="26.8984375" customWidth="1"/>
+    <col min="8" max="8" width="61.59765625" customWidth="1"/>
+    <col min="9" max="9" width="64.59765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.8984375" customWidth="1"/>
+    <col min="11" max="11" width="4.8984375" customWidth="1"/>
+    <col min="12" max="13" width="4.3984375" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="15" max="15" width="4.375" customWidth="1"/>
-    <col min="16" max="16" width="4.625" customWidth="1"/>
+    <col min="15" max="15" width="4.3984375" customWidth="1"/>
+    <col min="16" max="16" width="4.59765625" customWidth="1"/>
     <col min="17" max="17" width="42" customWidth="1"/>
-    <col min="18" max="18" width="3.125" customWidth="1"/>
-    <col min="19" max="19" width="3.375" customWidth="1"/>
-    <col min="20" max="20" width="44.125" customWidth="1"/>
-    <col min="21" max="21" width="15.625" customWidth="1"/>
+    <col min="18" max="18" width="3.09765625" customWidth="1"/>
+    <col min="19" max="19" width="3.3984375" customWidth="1"/>
+    <col min="20" max="20" width="44.09765625" customWidth="1"/>
+    <col min="21" max="21" width="15.59765625" customWidth="1"/>
     <col min="22" max="22" width="6.5" customWidth="1"/>
     <col min="23" max="23" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2960,200 +2973,200 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H2" s="2"/>
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H4" s="2"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H5" s="2"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H6" s="2"/>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H7" s="2"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H9" s="2"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H10" s="2"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H12" s="2"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H13" s="2"/>
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H15" s="2"/>
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H16" s="2"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="2"/>
       <c r="I17"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="2"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="2"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="2"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="2"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="2"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="2"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I24"/>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="2"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="2"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="2"/>
       <c r="I27"/>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I28"/>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I29"/>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="I30"/>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="2"/>
       <c r="I31"/>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="2"/>
       <c r="I32"/>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33" s="2"/>
       <c r="I33"/>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34" s="2"/>
       <c r="I34"/>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35" s="2"/>
       <c r="I35"/>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H36" s="2"/>
       <c r="I36"/>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H37" s="2"/>
       <c r="I37"/>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H38" s="2"/>
       <c r="I38"/>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39" s="2"/>
       <c r="I39"/>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H40" s="2"/>
       <c r="I40"/>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H41" s="2"/>
       <c r="I41"/>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H42" s="2"/>
       <c r="I42"/>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H43" s="2"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H44" s="2"/>
       <c r="I44"/>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H45" s="2"/>
       <c r="I45"/>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H46" s="2"/>
       <c r="I46"/>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H47" s="2"/>
       <c r="I47"/>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H48" s="2"/>
       <c r="I48"/>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H49" s="2"/>
       <c r="I49"/>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H50" s="2"/>
       <c r="I50"/>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H51" s="2"/>
       <c r="I51"/>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H52" s="2"/>
       <c r="I52"/>
     </row>
@@ -3167,21 +3180,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.375" customWidth="1"/>
-    <col min="2" max="2" width="35.625" customWidth="1"/>
-    <col min="3" max="3" width="168.625" customWidth="1"/>
+    <col min="1" max="1" width="25.3984375" customWidth="1"/>
+    <col min="2" max="2" width="35.59765625" customWidth="1"/>
+    <col min="3" max="3" width="168.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -3192,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3200,7 +3213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3208,7 +3221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3219,7 +3232,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3227,7 +3240,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -3235,7 +3248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -3243,7 +3256,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3251,7 +3264,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3259,7 +3272,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -3269,36 +3282,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.125" customWidth="1"/>
-    <col min="2" max="2" width="36.125" customWidth="1"/>
-    <col min="3" max="3" width="158.625" customWidth="1"/>
+    <col min="1" max="1" width="31.09765625" customWidth="1"/>
+    <col min="2" max="2" width="36.09765625" customWidth="1"/>
+    <col min="3" max="3" width="158.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -3309,7 +3322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3317,7 +3330,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -3325,7 +3338,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -3333,7 +3346,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -3341,7 +3354,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -3349,7 +3362,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -3357,7 +3370,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3365,7 +3378,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -3373,7 +3386,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -3381,107 +3394,125 @@
         <v>72</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{307FF3F5-9433-4D08-981D-ADE69EABA89D}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{13A3C325-A4DA-4730-B7BE-B467B8DD0C81}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3656,18 +3687,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Correction bug d'envoi de statement dans StoryDisplaying
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents HDD\LearningScape\LearningScape\Vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5FEEF2-62C1-4429-949B-A24F0E8EBA52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD2ADF1-0C81-411B-9B69-CA5CFE5E91A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t>URI</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>https://www.lip6.fr/mocah/invalidURI/extensions/scale</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/help</t>
   </si>
 </sst>
 </file>
@@ -3298,10 +3304,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3408,6 +3414,14 @@
       </c>
       <c r="B12" s="2" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3423,6 +3437,7 @@
     <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
     <hyperlink ref="B11" r:id="rId10" xr:uid="{307FF3F5-9433-4D08-981D-ADE69EABA89D}"/>
     <hyperlink ref="B12" r:id="rId11" xr:uid="{13A3C325-A4DA-4730-B7BE-B467B8DD0C81}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{6A1A847D-8861-4E26-978E-92D8AC3524D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3501,21 +3516,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002AF8BD77682A724D8C3CDE17EF043D04" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0bf18f5715a3c32625528aa9cf69777">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb470b12-e12f-4a6c-8c4e-b69976333524" xmlns:ns3="35b094a4-12a1-4fa9-8f69-05d08f840d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0ac61fa3f519b84257a19b7fcabbdac" ns2:_="" ns3:_="">
     <xsd:import namespace="bb470b12-e12f-4a6c-8c4e-b69976333524"/>
@@ -3686,24 +3686,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB0AA923-8FEF-4C78-9E38-5BD5DFE72B3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3720,4 +3718,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58977738-4157-4829-979D-9BDA401487A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D08F620C-FFEB-4C04-B37C-738A91901563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correction de bug du tableau effacable sur la version 2019 + sauvegarde et chargement des traces de Laalys
</commit_message>
<xml_diff>
--- a/Vocabulary/GBLxAPI_Vocab_User.xlsx
+++ b/Vocabulary/GBLxAPI_Vocab_User.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents HDD\LearningScape\LearningScape\Vocabulary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents HDD\LearningScape\LearningScape_2019\Vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5FEEF2-62C1-4429-949B-A24F0E8EBA52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A22DCC-EC7B-4B00-B4C3-0A680E391706}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verb" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
   <si>
     <t>URI</t>
   </si>
@@ -268,6 +268,24 @@
   </si>
   <si>
     <t>https://www.lip6.fr/mocah/invalidURI/extensions/scale</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/extensions/help</t>
+  </si>
+  <si>
+    <t>saved</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/saved</t>
+  </si>
+  <si>
+    <t>loaded</t>
+  </si>
+  <si>
+    <t>https://www.lip6.fr/mocah/invalidURI/verbs/loaded</t>
   </si>
 </sst>
 </file>
@@ -1194,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1345,6 +1363,22 @@
       </c>
       <c r="B16" s="2" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1364,6 +1398,8 @@
     <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{766B8C66-CF26-48C0-AB03-8F32DCB27D3F}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{6A34507C-CE11-4B4D-9669-C54BA132ED9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3298,10 +3334,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3408,6 +3444,14 @@
       </c>
       <c r="B12" s="2" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3423,6 +3467,7 @@
     <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
     <hyperlink ref="B11" r:id="rId10" xr:uid="{307FF3F5-9433-4D08-981D-ADE69EABA89D}"/>
     <hyperlink ref="B12" r:id="rId11" xr:uid="{13A3C325-A4DA-4730-B7BE-B467B8DD0C81}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{6A1A847D-8861-4E26-978E-92D8AC3524D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>